<commit_message>
doc + tests excel
</commit_message>
<xml_diff>
--- a/teste.xlsx
+++ b/teste.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="14355" windowHeight="4680"/>
+    <workbookView xWindow="360" yWindow="180" windowWidth="14355" windowHeight="4620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="29">
   <si>
     <t>Algoritm</t>
   </si>
@@ -124,6 +124,45 @@
   </si>
   <si>
     <t>mix2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>marja eroare</t>
+  </si>
+  <si>
+    <t>mix1-2</t>
+  </si>
+  <si>
+    <t>mix-34</t>
+  </si>
+  <si>
+    <t>idem</t>
+  </si>
+  <si>
+    <t>adam</t>
+  </si>
+  <si>
+    <t>9mixuri</t>
+  </si>
+  <si>
+    <t>3 de cate 1</t>
+  </si>
+  <si>
+    <t>4mixuri</t>
+  </si>
+  <si>
+    <t>mergea ok pe unele din train set</t>
+  </si>
+  <si>
+    <t>2 mixuri -80%</t>
+  </si>
+  <si>
+    <t>2 mixuri -10%</t>
+  </si>
+  <si>
+    <t>mergea bine pe cele din train, dar pe unele necunoscute gen test nu</t>
   </si>
 </sst>
 </file>
@@ -147,7 +186,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -178,6 +217,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -191,13 +236,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -499,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,9 +563,10 @@
     <col min="8" max="10" width="10.5703125" customWidth="1"/>
     <col min="11" max="11" width="11.85546875" customWidth="1"/>
     <col min="12" max="12" width="12.7109375" customWidth="1"/>
+    <col min="13" max="13" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
@@ -540,14 +588,17 @@
       <c r="J1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -576,7 +627,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -607,8 +658,11 @@
       <c r="J3" t="s">
         <v>14</v>
       </c>
+      <c r="K3" s="6">
+        <v>0.01</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -618,13 +672,13 @@
       <c r="C4">
         <v>1E-3</v>
       </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="D4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>15</v>
       </c>
       <c r="G4" s="5">
@@ -633,16 +687,19 @@
       <c r="H4" s="5">
         <v>0.92</v>
       </c>
-      <c r="I4" s="5">
-        <v>0.26</v>
+      <c r="I4" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="J4" t="s">
         <v>14</v>
       </c>
+      <c r="K4" s="6">
+        <v>0.01</v>
+      </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>7</v>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="B5">
         <v>200</v>
@@ -650,28 +707,204 @@
       <c r="C5">
         <v>1E-3</v>
       </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" t="s">
-        <v>8</v>
+      <c r="D5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="G5" s="5">
+        <v>0.98</v>
+      </c>
+      <c r="H5" s="5">
+        <v>0.95</v>
+      </c>
+      <c r="I5" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="J5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="6">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>500</v>
+      </c>
+      <c r="C6">
+        <v>1E-3</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="5">
+        <v>1</v>
+      </c>
+      <c r="H6" s="5">
+        <v>0.99</v>
+      </c>
+      <c r="I6" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="J6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="6">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>600</v>
+      </c>
+      <c r="C7">
+        <v>1E-3</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="5">
+        <v>0.74</v>
+      </c>
+      <c r="H7" s="5">
+        <v>0.68</v>
+      </c>
+      <c r="I7" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="J7" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8">
+        <v>800</v>
+      </c>
+      <c r="C8">
+        <v>1E-3</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9">
+        <v>400</v>
+      </c>
+      <c r="C9">
+        <v>1E-3</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="5">
+        <v>0.99</v>
+      </c>
+      <c r="H9" s="5">
+        <v>0.95</v>
+      </c>
+      <c r="I9" s="5">
+        <v>0.95</v>
+      </c>
+      <c r="J9" t="s">
+        <v>20</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>200</v>
+      </c>
+      <c r="C10">
+        <v>1E-3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="5">
         <v>0</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H10" s="5">
         <v>0</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I10" s="5">
         <v>0</v>
       </c>
-      <c r="K5">
+      <c r="K10" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="L10">
         <v>0.9</v>
       </c>
-      <c r="L5">
+      <c r="M10">
         <v>1E-4</v>
       </c>
     </row>

</xml_diff>